<commit_message>
Minor calcultion spreadsheet update for clarity
</commit_message>
<xml_diff>
--- a/doc/LFSR_Calculations.xlsx
+++ b/doc/LFSR_Calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Charley Lucas\work_hw\arty_e310\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E30FFAE-4416-4017-B9E6-BC87043CD3C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399C890A-5766-4AAF-89FF-5CCD70BB3D29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13305" yWindow="2610" windowWidth="38700" windowHeight="18165" activeTab="1" xr2:uid="{F88BD82E-167A-435E-9556-7854A5BDB32B}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="141">
   <si>
     <t>1SB2</t>
   </si>
@@ -218,18 +218,6 @@
   </si>
   <si>
     <t>7SB1</t>
-  </si>
-  <si>
-    <t>6 Step:</t>
-  </si>
-  <si>
-    <t>7 Step:</t>
-  </si>
-  <si>
-    <t>8 Step:</t>
-  </si>
-  <si>
-    <t>9 Step:</t>
   </si>
   <si>
     <t>6SB6</t>
@@ -468,13 +456,75 @@
 O7^
 O3</t>
   </si>
+  <si>
+    <t>BPC</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>B0</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -508,7 +558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -525,6 +575,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1028,11 +1081,11 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1040,92 +1093,95 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4999F10C-BEF5-4551-9CD0-556967C164DF}">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="17" max="17" width="13.85546875" customWidth="1"/>
-    <col min="18" max="18" width="16.140625" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" customWidth="1"/>
-    <col min="20" max="20" width="24.7109375" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" customWidth="1"/>
+    <col min="21" max="21" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" s="3">
         <v>0</v>
       </c>
+      <c r="K1" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="L1" s="3">
+        <v>0</v>
+      </c>
+      <c r="M1" s="3">
         <v>1</v>
       </c>
-      <c r="M1" s="3">
+      <c r="N1" s="3">
         <v>2</v>
       </c>
-      <c r="N1" s="3">
+      <c r="O1" s="3">
         <v>3</v>
       </c>
-      <c r="O1" s="3">
+      <c r="P1" s="3">
         <v>4</v>
       </c>
-      <c r="P1" s="3">
+      <c r="Q1" s="3">
         <v>5</v>
       </c>
-      <c r="Q1" s="3">
+      <c r="R1" s="3">
         <v>6</v>
       </c>
-      <c r="R1" s="3">
+      <c r="S1" s="3">
         <v>7</v>
       </c>
-      <c r="S1" s="3">
+      <c r="T1" s="3">
         <v>8</v>
       </c>
-      <c r="T1" s="3">
+      <c r="U1" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>18</v>
-      </c>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -1135,19 +1191,20 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
     </row>
-    <row r="3" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>59</v>
@@ -1165,51 +1222,54 @@
         <v>1</v>
       </c>
       <c r="J3" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>105</v>
+      <c r="Q3" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>114</v>
+        <v>101</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>60</v>
@@ -1227,51 +1287,54 @@
         <v>0</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>105</v>
+      <c r="R4" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>111</v>
+        <v>101</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>61</v>
@@ -1289,48 +1352,51 @@
         <v>2</v>
       </c>
       <c r="J5" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="M5" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="O5" s="5" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>121</v>
+        <v>108</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>124</v>
+        <v>117</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>62</v>
@@ -1351,51 +1417,54 @@
         <v>3</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="M6" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="O6" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="N6" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>110</v>
-      </c>
       <c r="P6" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="T6" s="5" t="s">
-        <v>125</v>
+        <v>112</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>40</v>
@@ -1413,51 +1482,54 @@
         <v>4</v>
       </c>
       <c r="J7" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>105</v>
+      <c r="M7" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>114</v>
+        <v>101</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="T7" s="6" t="s">
-        <v>126</v>
+        <v>116</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>41</v>
@@ -1475,51 +1547,54 @@
         <v>5</v>
       </c>
       <c r="J8" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>105</v>
+      <c r="N8" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>114</v>
+        <v>101</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="T8" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>42</v>
@@ -1537,51 +1612,54 @@
         <v>6</v>
       </c>
       <c r="J9" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="K9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N9" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>105</v>
+      <c r="O9" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="R9" s="5" t="s">
-        <v>114</v>
+        <v>101</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="S9" s="5" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>120</v>
+        <v>113</v>
+      </c>
+      <c r="U9" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>44</v>
@@ -1599,46 +1677,49 @@
         <v>7</v>
       </c>
       <c r="J10" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="O10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O10" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="P10" s="5" t="s">
-        <v>105</v>
+      <c r="P10" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="R10" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="S10" s="5" t="s">
-        <v>114</v>
+        <v>101</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="S10" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="T10" s="5" t="s">
-        <v>117</v>
+        <v>110</v>
+      </c>
+      <c r="U10" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>